<commit_message>
updated MAPs with new response model
</commit_message>
<xml_diff>
--- a/PreprocessingAnalysis/wagad_MAPs.xlsx
+++ b/PreprocessingAnalysis/wagad_MAPs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/drea/Dropbox/MadelineMSc/Code/WAGAD/PreprocessingAnalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFEC71E0-8D0C-174B-9A7B-A7EAA619C619}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{700750C9-D0E8-E847-A0AD-B410A6B89D24}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="460" windowWidth="27820" windowHeight="17040" activeTab="1" xr2:uid="{8AF74A6B-C1C0-BD44-B75B-082213368F0D}"/>
   </bookViews>
@@ -67,23 +67,43 @@
     <definedName name="_xlchart.v1.51" hidden="1">Sheet1!$G$2:$G$41</definedName>
     <definedName name="_xlchart.v1.52" hidden="1">Sheet1!$P$1</definedName>
     <definedName name="_xlchart.v1.53" hidden="1">Sheet1!$P$2:$P$41</definedName>
-    <definedName name="_xlchart.v1.54" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.55" hidden="1">Sheet1!$B$2:$B$41</definedName>
-    <definedName name="_xlchart.v1.56" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.57" hidden="1">Sheet1!$C$2:$C$41</definedName>
-    <definedName name="_xlchart.v1.58" hidden="1">Sheet1!$D$1</definedName>
-    <definedName name="_xlchart.v1.59" hidden="1">Sheet1!$D$2:$D$41</definedName>
+    <definedName name="_xlchart.v1.54" hidden="1">Sheet1!$C$1</definedName>
+    <definedName name="_xlchart.v1.55" hidden="1">Sheet1!$C$2:$C$41</definedName>
+    <definedName name="_xlchart.v1.56" hidden="1">Sheet1!$D$1</definedName>
+    <definedName name="_xlchart.v1.57" hidden="1">Sheet1!$D$2:$D$41</definedName>
+    <definedName name="_xlchart.v1.58" hidden="1">Sheet1!$E$1</definedName>
+    <definedName name="_xlchart.v1.59" hidden="1">Sheet1!$E$2:$E$41</definedName>
     <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$F$1</definedName>
-    <definedName name="_xlchart.v1.60" hidden="1">Sheet1!$E$1</definedName>
-    <definedName name="_xlchart.v1.61" hidden="1">Sheet1!$E$2:$E$41</definedName>
-    <definedName name="_xlchart.v1.62" hidden="1">Sheet1!$F$1</definedName>
-    <definedName name="_xlchart.v1.63" hidden="1">Sheet1!$F$2:$F$41</definedName>
-    <definedName name="_xlchart.v1.64" hidden="1">Sheet1!$G$1</definedName>
-    <definedName name="_xlchart.v1.65" hidden="1">Sheet1!$G$2:$G$41</definedName>
-    <definedName name="_xlchart.v1.66" hidden="1">Sheet1!$P$1</definedName>
-    <definedName name="_xlchart.v1.67" hidden="1">Sheet1!$P$2:$P$41</definedName>
+    <definedName name="_xlchart.v1.60" hidden="1">Sheet1!$F$1</definedName>
+    <definedName name="_xlchart.v1.61" hidden="1">Sheet1!$F$2:$F$41</definedName>
+    <definedName name="_xlchart.v1.62" hidden="1">Sheet1!$G$1</definedName>
+    <definedName name="_xlchart.v1.63" hidden="1">Sheet1!$G$2:$G$41</definedName>
+    <definedName name="_xlchart.v1.64" hidden="1">Sheet1!$C$1</definedName>
+    <definedName name="_xlchart.v1.65" hidden="1">Sheet1!$C$2:$C$41</definedName>
+    <definedName name="_xlchart.v1.66" hidden="1">Sheet1!$D$1</definedName>
+    <definedName name="_xlchart.v1.67" hidden="1">Sheet1!$D$2:$D$41</definedName>
+    <definedName name="_xlchart.v1.68" hidden="1">Sheet1!$E$1</definedName>
+    <definedName name="_xlchart.v1.69" hidden="1">Sheet1!$E$2:$E$41</definedName>
     <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$F$2:$F$41</definedName>
+    <definedName name="_xlchart.v1.70" hidden="1">Sheet1!$F$1</definedName>
+    <definedName name="_xlchart.v1.71" hidden="1">Sheet1!$F$2:$F$41</definedName>
+    <definedName name="_xlchart.v1.72" hidden="1">Sheet1!$G$1</definedName>
+    <definedName name="_xlchart.v1.73" hidden="1">Sheet1!$G$2:$G$41</definedName>
+    <definedName name="_xlchart.v1.74" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.75" hidden="1">Sheet1!$B$2:$B$41</definedName>
+    <definedName name="_xlchart.v1.76" hidden="1">Sheet1!$C$1</definedName>
+    <definedName name="_xlchart.v1.77" hidden="1">Sheet1!$C$2:$C$41</definedName>
+    <definedName name="_xlchart.v1.78" hidden="1">Sheet1!$D$1</definedName>
+    <definedName name="_xlchart.v1.79" hidden="1">Sheet1!$D$2:$D$41</definedName>
     <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$G$1</definedName>
+    <definedName name="_xlchart.v1.80" hidden="1">Sheet1!$E$1</definedName>
+    <definedName name="_xlchart.v1.81" hidden="1">Sheet1!$E$2:$E$41</definedName>
+    <definedName name="_xlchart.v1.82" hidden="1">Sheet1!$F$1</definedName>
+    <definedName name="_xlchart.v1.83" hidden="1">Sheet1!$F$2:$F$41</definedName>
+    <definedName name="_xlchart.v1.84" hidden="1">Sheet1!$G$1</definedName>
+    <definedName name="_xlchart.v1.85" hidden="1">Sheet1!$G$2:$G$41</definedName>
+    <definedName name="_xlchart.v1.86" hidden="1">Sheet1!$P$1</definedName>
+    <definedName name="_xlchart.v1.87" hidden="1">Sheet1!$P$2:$P$41</definedName>
     <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$G$2:$G$41</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -243,48 +263,38 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.13</cx:f>
+        <cx:f>_xlchart.v1.15</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.15</cx:f>
+        <cx:f>_xlchart.v1.17</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.17</cx:f>
+        <cx:f>_xlchart.v1.19</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.19</cx:f>
+        <cx:f>_xlchart.v1.21</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="4">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.21</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="5">
-      <cx:numDim type="val">
         <cx:f>_xlchart.v1.23</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="6">
-      <cx:numDim type="val">
-        <cx:f>_xlchart.v1.25</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
   <cx:chart>
     <cx:plotArea>
       <cx:plotAreaRegion>
-        <cx:series layoutId="boxWhisker" uniqueId="{ECA32619-D88E-1D4F-A164-66F43104E1C7}">
+        <cx:series layoutId="boxWhisker" uniqueId="{5F28556B-1B99-1042-9190-C180E10E9A96}" formatIdx="1">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.12</cx:f>
-              <cx:v>surp</cx:v>
+              <cx:f>_xlchart.v1.14</cx:f>
+              <cx:v>arbitration</cx:v>
             </cx:txData>
           </cx:tx>
           <cx:dataId val="0"/>
@@ -293,11 +303,11 @@
             <cx:statistics quartileMethod="exclusive"/>
           </cx:layoutPr>
         </cx:series>
-        <cx:series layoutId="boxWhisker" uniqueId="{5F28556B-1B99-1042-9190-C180E10E9A96}">
+        <cx:series layoutId="boxWhisker" uniqueId="{F6E9F9BA-7CA1-DF44-B69F-A8C4205DDD6B}" formatIdx="2">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.14</cx:f>
-              <cx:v>arbitration</cx:v>
+              <cx:f>_xlchart.v1.16</cx:f>
+              <cx:v>inf_a</cx:v>
             </cx:txData>
           </cx:tx>
           <cx:dataId val="1"/>
@@ -306,11 +316,11 @@
             <cx:statistics quartileMethod="exclusive"/>
           </cx:layoutPr>
         </cx:series>
-        <cx:series layoutId="boxWhisker" uniqueId="{F6E9F9BA-7CA1-DF44-B69F-A8C4205DDD6B}">
+        <cx:series layoutId="boxWhisker" uniqueId="{C1B763A0-6323-9C41-967C-E772791F58D6}" formatIdx="3">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.16</cx:f>
-              <cx:v>inf_a</cx:v>
+              <cx:f>_xlchart.v1.18</cx:f>
+              <cx:v>inf_r</cx:v>
             </cx:txData>
           </cx:tx>
           <cx:dataId val="2"/>
@@ -319,11 +329,11 @@
             <cx:statistics quartileMethod="exclusive"/>
           </cx:layoutPr>
         </cx:series>
-        <cx:series layoutId="boxWhisker" uniqueId="{C1B763A0-6323-9C41-967C-E772791F58D6}">
+        <cx:series layoutId="boxWhisker" uniqueId="{24E9C62D-4993-3C49-94B5-1373C4D5EC18}" formatIdx="4">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.18</cx:f>
-              <cx:v>inf_r</cx:v>
+              <cx:f>_xlchart.v1.20</cx:f>
+              <cx:v>vol_a</cx:v>
             </cx:txData>
           </cx:tx>
           <cx:dataId val="3"/>
@@ -332,40 +342,14 @@
             <cx:statistics quartileMethod="exclusive"/>
           </cx:layoutPr>
         </cx:series>
-        <cx:series layoutId="boxWhisker" uniqueId="{24E9C62D-4993-3C49-94B5-1373C4D5EC18}">
-          <cx:tx>
-            <cx:txData>
-              <cx:f>_xlchart.v1.20</cx:f>
-              <cx:v>vol_a</cx:v>
-            </cx:txData>
-          </cx:tx>
-          <cx:dataId val="4"/>
-          <cx:layoutPr>
-            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
-            <cx:statistics quartileMethod="exclusive"/>
-          </cx:layoutPr>
-        </cx:series>
-        <cx:series layoutId="boxWhisker" uniqueId="{1873B201-F31E-8741-94AF-126973653FD4}">
+        <cx:series layoutId="boxWhisker" uniqueId="{1873B201-F31E-8741-94AF-126973653FD4}" formatIdx="5">
           <cx:tx>
             <cx:txData>
               <cx:f>_xlchart.v1.22</cx:f>
               <cx:v>vol_r</cx:v>
             </cx:txData>
           </cx:tx>
-          <cx:dataId val="5"/>
-          <cx:layoutPr>
-            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
-            <cx:statistics quartileMethod="exclusive"/>
-          </cx:layoutPr>
-        </cx:series>
-        <cx:series layoutId="boxWhisker" uniqueId="{C958C876-6BFA-F84D-9E95-C8DDE4815B23}">
-          <cx:tx>
-            <cx:txData>
-              <cx:f>_xlchart.v1.24</cx:f>
-              <cx:v>logZeta</cx:v>
-            </cx:txData>
-          </cx:tx>
-          <cx:dataId val="6"/>
+          <cx:dataId val="4"/>
           <cx:layoutPr>
             <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
             <cx:statistics quartileMethod="exclusive"/>
@@ -375,6 +359,25 @@
       <cx:axis id="0">
         <cx:catScaling gapWidth="1.5"/>
         <cx:tickLabels/>
+        <cx:txPr>
+          <a:bodyPr vertOverflow="overflow" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr" rtl="0">
+              <a:defRPr sz="2000" b="0">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Constantia" panose="02030602050306030303" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Constantia" panose="02030602050306030303" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Constantia" panose="02030602050306030303" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US" sz="2000">
+              <a:latin typeface="Constantia" panose="02030602050306030303" pitchFamily="18" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </cx:txPr>
       </cx:axis>
       <cx:axis id="1">
         <cx:valScaling/>
@@ -386,16 +389,20 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr" rtl="0">
-              <a:defRPr sz="2400"/>
+              <a:defRPr sz="2000">
+                <a:latin typeface="Constantia" panose="02030602050306030303" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Constantia" panose="02030602050306030303" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Constantia" panose="02030602050306030303" pitchFamily="18" charset="0"/>
+              </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US" sz="2400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:endParaRPr lang="en-US" sz="2000" b="0" i="0" u="none" strike="noStrike" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
                 </a:sysClr>
               </a:solidFill>
-              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              <a:latin typeface="Constantia" panose="02030602050306030303" pitchFamily="18" charset="0"/>
             </a:endParaRPr>
           </a:p>
         </cx:txPr>
@@ -403,20 +410,21 @@
     </cx:plotArea>
     <cx:legend pos="r" align="ctr" overlay="0">
       <cx:txPr>
-        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:bodyPr vertOverflow="overflow" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0"/>
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="ctr" rtl="0">
-            <a:defRPr sz="1200"/>
+            <a:defRPr sz="2000" b="0">
+              <a:solidFill>
+                <a:srgbClr val="595959"/>
+              </a:solidFill>
+              <a:latin typeface="Constantia" panose="02030602050306030303" pitchFamily="18" charset="0"/>
+              <a:ea typeface="Constantia" panose="02030602050306030303" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Constantia" panose="02030602050306030303" pitchFamily="18" charset="0"/>
+            </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-            <a:solidFill>
-              <a:sysClr val="windowText" lastClr="000000">
-                <a:lumMod val="65000"/>
-                <a:lumOff val="35000"/>
-              </a:sysClr>
-            </a:solidFill>
-            <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+          <a:endParaRPr lang="en-US" sz="2000">
+            <a:latin typeface="Constantia" panose="02030602050306030303" pitchFamily="18" charset="0"/>
           </a:endParaRPr>
         </a:p>
       </cx:txPr>
@@ -990,10 +998,10 @@
       <xdr:rowOff>196850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>292100</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -1030,7 +1038,7 @@
           <xdr:spPr>
             <a:xfrm>
               <a:off x="2590800" y="2635250"/>
-              <a:ext cx="9398000" cy="5124450"/>
+              <a:ext cx="7416800" cy="5175250"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>

</xml_diff>